<commit_message>
added cleaner.py, convertor.py, type_schemas.py
</commit_message>
<xml_diff>
--- a/data/raw/sample_cleaned.xlsx
+++ b/data/raw/sample_cleaned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Dev_job\excel_parser_openpyxl_only\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0BAAD0-229D-478F-A26C-99A131C1EE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BA1721-B652-4E0C-AB6F-B15EF54C3144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31170" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45" yWindow="105" windowWidth="31170" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="РЕГЛАМЕНТ" sheetId="1" r:id="rId1"/>
@@ -6365,25 +6365,25 @@
     <xf numFmtId="0" fontId="1" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6734,10 +6734,10 @@
   <dimension ref="B1:AF471"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="3" topLeftCell="T270" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="3" topLeftCell="K4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A304" sqref="A304"/>
-      <selection pane="bottomRight" activeCell="AF1" sqref="AF1"/>
+      <selection pane="bottomRight" activeCell="AF466" sqref="AF466"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6775,7 +6775,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" s="11" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="190" t="s">
+      <c r="B1" s="184" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="185"/>
@@ -6793,7 +6793,7 @@
         <v>2</v>
       </c>
       <c r="K1" s="186"/>
-      <c r="L1" s="189" t="s">
+      <c r="L1" s="191" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="186"/>
@@ -6816,7 +6816,7 @@
       </c>
       <c r="U1" s="14">
         <f ca="1">TODAY()</f>
-        <v>45783</v>
+        <v>45784</v>
       </c>
       <c r="W1" s="15"/>
     </row>
@@ -6840,22 +6840,22 @@
       <c r="O2" s="21"/>
       <c r="R2" s="22"/>
       <c r="S2" s="10"/>
-      <c r="T2" s="184" t="s">
+      <c r="T2" s="189" t="s">
         <v>9</v>
       </c>
       <c r="U2" s="185"/>
       <c r="V2" s="186"/>
-      <c r="W2" s="191" t="s">
+      <c r="W2" s="188" t="s">
         <v>10</v>
       </c>
       <c r="X2" s="185"/>
       <c r="Y2" s="186"/>
-      <c r="Z2" s="184" t="s">
+      <c r="Z2" s="189" t="s">
         <v>11</v>
       </c>
       <c r="AA2" s="185"/>
       <c r="AB2" s="186"/>
-      <c r="AC2" s="188" t="s">
+      <c r="AC2" s="190" t="s">
         <v>12</v>
       </c>
       <c r="AD2" s="185"/>
@@ -7817,7 +7817,7 @@
       </c>
       <c r="AE13" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>1638.5</v>
+        <v>1637.5</v>
       </c>
     </row>
     <row r="14" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -8329,7 +8329,7 @@
       </c>
       <c r="AE19" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>5291</v>
+        <v>5290</v>
       </c>
     </row>
     <row r="20" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -8501,7 +8501,7 @@
       </c>
       <c r="AE21" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>1638.5</v>
+        <v>1637.5</v>
       </c>
     </row>
     <row r="22" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -8587,7 +8587,7 @@
       </c>
       <c r="AE22" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>1638.5</v>
+        <v>1637.5</v>
       </c>
     </row>
     <row r="23" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -8675,7 +8675,7 @@
       </c>
       <c r="AE23" s="91">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>1638.5</v>
+        <v>1637.5</v>
       </c>
       <c r="AF23" s="93" t="s">
         <v>156</v>
@@ -8852,7 +8852,7 @@
       </c>
       <c r="AE25" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="26" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -8942,7 +8942,7 @@
       </c>
       <c r="AE26" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="27" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -9030,7 +9030,7 @@
       </c>
       <c r="AE27" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="28" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -9120,7 +9120,7 @@
       </c>
       <c r="AE28" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="29" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -9210,7 +9210,7 @@
       </c>
       <c r="AE29" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="30" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -9300,7 +9300,7 @@
       </c>
       <c r="AE30" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="31" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -9384,7 +9384,7 @@
       </c>
       <c r="AE31" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>1638.5</v>
+        <v>1637.5</v>
       </c>
     </row>
     <row r="32" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -9470,7 +9470,7 @@
       </c>
       <c r="AE32" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>1638.5</v>
+        <v>1637.5</v>
       </c>
     </row>
     <row r="33" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -9566,7 +9566,7 @@
       </c>
       <c r="AE33" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="34" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -9662,7 +9662,7 @@
       </c>
       <c r="AE34" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="35" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -9760,7 +9760,7 @@
       </c>
       <c r="AE35" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="36" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -9856,7 +9856,7 @@
       </c>
       <c r="AE36" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="37" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -9952,7 +9952,7 @@
       </c>
       <c r="AE37" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="38" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -10048,7 +10048,7 @@
       </c>
       <c r="AE38" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="39" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -10144,7 +10144,7 @@
       </c>
       <c r="AE39" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="40" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -10240,7 +10240,7 @@
       </c>
       <c r="AE40" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="41" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -10336,7 +10336,7 @@
       </c>
       <c r="AE41" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="42" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -10432,7 +10432,7 @@
       </c>
       <c r="AE42" s="71">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>-130.75</v>
+        <v>-131.75</v>
       </c>
       <c r="AF42" s="108" t="s">
         <v>107</v>
@@ -10531,7 +10531,7 @@
       </c>
       <c r="AE43" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="44" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -10627,7 +10627,7 @@
       </c>
       <c r="AE44" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="45" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -10723,7 +10723,7 @@
       </c>
       <c r="AE45" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="46" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -10819,7 +10819,7 @@
       </c>
       <c r="AE46" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="47" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -10915,7 +10915,7 @@
       </c>
       <c r="AE47" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="48" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -11011,7 +11011,7 @@
       </c>
       <c r="AE48" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="49" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -11107,7 +11107,7 @@
       </c>
       <c r="AE49" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="50" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -11205,7 +11205,7 @@
       </c>
       <c r="AE50" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="51" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -11303,7 +11303,7 @@
       </c>
       <c r="AE51" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="52" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -11399,7 +11399,7 @@
       </c>
       <c r="AE52" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="53" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -11497,7 +11497,7 @@
       </c>
       <c r="AE53" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="54" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -11589,7 +11589,7 @@
       </c>
       <c r="AE54" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="55" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -11685,7 +11685,7 @@
       </c>
       <c r="AE55" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="56" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -11781,7 +11781,7 @@
       </c>
       <c r="AE56" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="57" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -11877,7 +11877,7 @@
       </c>
       <c r="AE57" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="58" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -11973,7 +11973,7 @@
       </c>
       <c r="AE58" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="59" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -12069,7 +12069,7 @@
       </c>
       <c r="AE59" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="60" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -12165,7 +12165,7 @@
       </c>
       <c r="AE60" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="61" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -12261,7 +12261,7 @@
       </c>
       <c r="AE61" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="62" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -12357,7 +12357,7 @@
       </c>
       <c r="AE62" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="63" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -12453,7 +12453,7 @@
       </c>
       <c r="AE63" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="64" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -12551,7 +12551,7 @@
       </c>
       <c r="AE64" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="65" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -12647,7 +12647,7 @@
       </c>
       <c r="AE65" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="66" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -12743,7 +12743,7 @@
       </c>
       <c r="AE66" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="67" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -12839,7 +12839,7 @@
       </c>
       <c r="AE67" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="68" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -12935,7 +12935,7 @@
       </c>
       <c r="AE68" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="69" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -13031,7 +13031,7 @@
       </c>
       <c r="AE69" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="70" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -13394,7 +13394,7 @@
       </c>
       <c r="AE73" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="74" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -13490,7 +13490,7 @@
       </c>
       <c r="AE74" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="75" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -13586,7 +13586,7 @@
       </c>
       <c r="AE75" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="76" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -13682,7 +13682,7 @@
       </c>
       <c r="AE76" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="77" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -13778,7 +13778,7 @@
       </c>
       <c r="AE77" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="78" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -13963,7 +13963,7 @@
       </c>
       <c r="AE79" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="80" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -14059,7 +14059,7 @@
       </c>
       <c r="AE80" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="81" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -14155,7 +14155,7 @@
       </c>
       <c r="AE81" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="82" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -14251,7 +14251,7 @@
       </c>
       <c r="AE82" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="83" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -14347,7 +14347,7 @@
       </c>
       <c r="AE83" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="84" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -14443,7 +14443,7 @@
       </c>
       <c r="AE84" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="85" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -14539,7 +14539,7 @@
       </c>
       <c r="AE85" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="86" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -14635,7 +14635,7 @@
       </c>
       <c r="AE86" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="87" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -14731,7 +14731,7 @@
       </c>
       <c r="AE87" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="88" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -14827,7 +14827,7 @@
       </c>
       <c r="AE88" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="89" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -14923,7 +14923,7 @@
       </c>
       <c r="AE89" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="90" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -15019,7 +15019,7 @@
       </c>
       <c r="AE90" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="91" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -15115,7 +15115,7 @@
       </c>
       <c r="AE91" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="92" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -15211,7 +15211,7 @@
       </c>
       <c r="AE92" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="93" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -15307,7 +15307,7 @@
       </c>
       <c r="AE93" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="94" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -15403,7 +15403,7 @@
       </c>
       <c r="AE94" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="95" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -15499,7 +15499,7 @@
       </c>
       <c r="AE95" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="96" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -15595,7 +15595,7 @@
       </c>
       <c r="AE96" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="97" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -15691,7 +15691,7 @@
       </c>
       <c r="AE97" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="98" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -15789,7 +15789,7 @@
       </c>
       <c r="AE98" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="99" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -15887,7 +15887,7 @@
       </c>
       <c r="AE99" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="100" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -15985,7 +15985,7 @@
       </c>
       <c r="AE100" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="101" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -16083,7 +16083,7 @@
       </c>
       <c r="AE101" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="102" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -16175,7 +16175,7 @@
       </c>
       <c r="AE102" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
       <c r="AF102" t="str">
         <f>(Таблица1[[#This Row],[Next  F.H.]]+0.1*Таблица1[[#This Row],[F.H.]])&amp;" "&amp;"F.H. DEADLINE. Remain"&amp;" "&amp;((Таблица1[[#This Row],[Next  F.H.]]+0.1*Таблица1[[#This Row],[F.H.]])-$P$1)&amp;" "&amp;"F.H."</f>
@@ -16701,7 +16701,7 @@
       </c>
       <c r="AE108" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>2369</v>
+        <v>2368</v>
       </c>
     </row>
     <row r="109" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -16787,7 +16787,7 @@
       </c>
       <c r="AE109" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>1638.5</v>
+        <v>1637.5</v>
       </c>
     </row>
     <row r="110" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -17043,7 +17043,7 @@
       </c>
       <c r="AE112" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>3464.75</v>
+        <v>3463.75</v>
       </c>
     </row>
     <row r="113" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -17135,7 +17135,7 @@
       </c>
       <c r="AE113" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="114" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -17227,7 +17227,7 @@
       </c>
       <c r="AE114" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="115" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -17319,7 +17319,7 @@
       </c>
       <c r="AE115" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="116" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -17411,7 +17411,7 @@
       </c>
       <c r="AE116" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="117" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -17503,7 +17503,7 @@
       </c>
       <c r="AE117" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="118" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -17595,7 +17595,7 @@
       </c>
       <c r="AE118" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="119" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -17775,7 +17775,7 @@
       </c>
       <c r="AE120" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="121" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -17867,7 +17867,7 @@
       </c>
       <c r="AE121" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="122" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -17959,7 +17959,7 @@
       </c>
       <c r="AE122" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="123" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -18387,7 +18387,7 @@
       </c>
       <c r="AE127" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>599.5</v>
+        <v>598.5</v>
       </c>
     </row>
     <row r="128" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -18477,7 +18477,7 @@
       </c>
       <c r="AE128" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>599.5</v>
+        <v>598.5</v>
       </c>
     </row>
     <row r="129" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -18567,7 +18567,7 @@
       </c>
       <c r="AE129" s="71">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>-179.5</v>
+        <v>-180.5</v>
       </c>
       <c r="AF129" s="125" t="s">
         <v>107</v>
@@ -18660,7 +18660,7 @@
       </c>
       <c r="AE130" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>599.5</v>
+        <v>598.5</v>
       </c>
     </row>
     <row r="131" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -18750,7 +18750,7 @@
       </c>
       <c r="AE131" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>599.5</v>
+        <v>598.5</v>
       </c>
     </row>
     <row r="132" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -18840,7 +18840,7 @@
       </c>
       <c r="AE132" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>599.5</v>
+        <v>598.5</v>
       </c>
     </row>
     <row r="133" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -18932,7 +18932,7 @@
       </c>
       <c r="AE133" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="134" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -19030,7 +19030,7 @@
       </c>
       <c r="AE134" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="135" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -19126,7 +19126,7 @@
       </c>
       <c r="AE135" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="136" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -19222,7 +19222,7 @@
       </c>
       <c r="AE136" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="137" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -19318,7 +19318,7 @@
       </c>
       <c r="AE137" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="138" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -19414,7 +19414,7 @@
       </c>
       <c r="AE138" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="139" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -19510,7 +19510,7 @@
       </c>
       <c r="AE139" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="140" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -19606,7 +19606,7 @@
       </c>
       <c r="AE140" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="141" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -19702,7 +19702,7 @@
       </c>
       <c r="AE141" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="142" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -19798,7 +19798,7 @@
       </c>
       <c r="AE142" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="143" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -19896,7 +19896,7 @@
       </c>
       <c r="AE143" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="144" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -19992,7 +19992,7 @@
       </c>
       <c r="AE144" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="145" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -20088,7 +20088,7 @@
       </c>
       <c r="AE145" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="146" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -20184,7 +20184,7 @@
       </c>
       <c r="AE146" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="147" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -20280,7 +20280,7 @@
       </c>
       <c r="AE147" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="148" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -20376,7 +20376,7 @@
       </c>
       <c r="AE148" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="149" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -20472,7 +20472,7 @@
       </c>
       <c r="AE149" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="150" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -20568,7 +20568,7 @@
       </c>
       <c r="AE150" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="151" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -20662,7 +20662,7 @@
       </c>
       <c r="AE151" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="152" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -20756,7 +20756,7 @@
       </c>
       <c r="AE152" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="153" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -20852,7 +20852,7 @@
       </c>
       <c r="AE153" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="154" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -20946,7 +20946,7 @@
       </c>
       <c r="AE154" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="155" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -21040,7 +21040,7 @@
       </c>
       <c r="AE155" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="156" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -21136,7 +21136,7 @@
       </c>
       <c r="AE156" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="157" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -21232,7 +21232,7 @@
       </c>
       <c r="AE157" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="158" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -21417,7 +21417,7 @@
       </c>
       <c r="AE159" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="160" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -21513,7 +21513,7 @@
       </c>
       <c r="AE160" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="161" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -21609,7 +21609,7 @@
       </c>
       <c r="AE161" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="162" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -21705,7 +21705,7 @@
       </c>
       <c r="AE162" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="163" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -21801,7 +21801,7 @@
       </c>
       <c r="AE163" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="164" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -21895,7 +21895,7 @@
       </c>
       <c r="AE164" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.5</v>
+        <v>233.5</v>
       </c>
     </row>
     <row r="165" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -22429,7 +22429,7 @@
       </c>
       <c r="AE170" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="171" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -22525,7 +22525,7 @@
       </c>
       <c r="AE171" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="172" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -22621,7 +22621,7 @@
       </c>
       <c r="AE172" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="173" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -22717,7 +22717,7 @@
       </c>
       <c r="AE173" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="174" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -22813,7 +22813,7 @@
       </c>
       <c r="AE174" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="175" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -22909,7 +22909,7 @@
       </c>
       <c r="AE175" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="176" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -23007,7 +23007,7 @@
       </c>
       <c r="AE176" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="177" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -23103,7 +23103,7 @@
       </c>
       <c r="AE177" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="178" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -23199,7 +23199,7 @@
       </c>
       <c r="AE178" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="179" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -23295,7 +23295,7 @@
       </c>
       <c r="AE179" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="180" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -23391,7 +23391,7 @@
       </c>
       <c r="AE180" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="181" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -23485,7 +23485,7 @@
       </c>
       <c r="AE181" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="182" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -23581,7 +23581,7 @@
       </c>
       <c r="AE182" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="183" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -23677,7 +23677,7 @@
       </c>
       <c r="AE183" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="184" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -23773,7 +23773,7 @@
       </c>
       <c r="AE184" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="185" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -23869,7 +23869,7 @@
       </c>
       <c r="AE185" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="186" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -23965,7 +23965,7 @@
       </c>
       <c r="AE186" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="187" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -24061,7 +24061,7 @@
       </c>
       <c r="AE187" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="188" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -24157,7 +24157,7 @@
       </c>
       <c r="AE188" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="189" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -24253,7 +24253,7 @@
       </c>
       <c r="AE189" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="190" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -24349,7 +24349,7 @@
       </c>
       <c r="AE190" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="191" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -24445,7 +24445,7 @@
       </c>
       <c r="AE191" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="192" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -24541,7 +24541,7 @@
       </c>
       <c r="AE192" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="193" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -24819,7 +24819,7 @@
       </c>
       <c r="AE195" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="196" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -24915,7 +24915,7 @@
       </c>
       <c r="AE196" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="197" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -25011,7 +25011,7 @@
       </c>
       <c r="AE197" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="198" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -25107,7 +25107,7 @@
       </c>
       <c r="AE198" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="199" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -25205,7 +25205,7 @@
       </c>
       <c r="AE199" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="200" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -25301,7 +25301,7 @@
       </c>
       <c r="AE200" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="201" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -25397,7 +25397,7 @@
       </c>
       <c r="AE201" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="202" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -25493,7 +25493,7 @@
       </c>
       <c r="AE202" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="203" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -25589,7 +25589,7 @@
       </c>
       <c r="AE203" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="204" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -25685,7 +25685,7 @@
       </c>
       <c r="AE204" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="205" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -25781,7 +25781,7 @@
       </c>
       <c r="AE205" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="206" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -25877,7 +25877,7 @@
       </c>
       <c r="AE206" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="207" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -25973,7 +25973,7 @@
       </c>
       <c r="AE207" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="208" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -26069,7 +26069,7 @@
       </c>
       <c r="AE208" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="209" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -26165,7 +26165,7 @@
       </c>
       <c r="AE209" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="210" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -26261,7 +26261,7 @@
       </c>
       <c r="AE210" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="211" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -26357,7 +26357,7 @@
       </c>
       <c r="AE211" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="212" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -26453,7 +26453,7 @@
       </c>
       <c r="AE212" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="213" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -26551,7 +26551,7 @@
       </c>
       <c r="AE213" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="214" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -26645,7 +26645,7 @@
       </c>
       <c r="AE214" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="215" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -26743,7 +26743,7 @@
       </c>
       <c r="AE215" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="216" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -26839,7 +26839,7 @@
       </c>
       <c r="AE216" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="217" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -26935,7 +26935,7 @@
       </c>
       <c r="AE217" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="218" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -27031,7 +27031,7 @@
       </c>
       <c r="AE218" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="219" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -27127,7 +27127,7 @@
       </c>
       <c r="AE219" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="220" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -27223,7 +27223,7 @@
       </c>
       <c r="AE220" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="221" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -27319,7 +27319,7 @@
       </c>
       <c r="AE221" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="222" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -27415,7 +27415,7 @@
       </c>
       <c r="AE222" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="223" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -27511,7 +27511,7 @@
       </c>
       <c r="AE223" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="224" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -27607,7 +27607,7 @@
       </c>
       <c r="AE224" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="225" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -27701,7 +27701,7 @@
       </c>
       <c r="AE225" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="226" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -29021,7 +29021,7 @@
       </c>
       <c r="AE239" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="240" spans="2:32" s="131" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -29198,7 +29198,7 @@
       </c>
       <c r="AE241" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="242" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -29290,7 +29290,7 @@
       </c>
       <c r="AE242" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="243" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -29382,7 +29382,7 @@
       </c>
       <c r="AE243" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="244" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -29474,7 +29474,7 @@
       </c>
       <c r="AE244" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="245" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -29986,7 +29986,7 @@
       </c>
       <c r="AE250" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>185.75</v>
+        <v>184.75</v>
       </c>
     </row>
     <row r="251" spans="2:32" s="131" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -30167,7 +30167,7 @@
       </c>
       <c r="AE252" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="253" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -30261,7 +30261,7 @@
       </c>
       <c r="AE253" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="254" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -30355,7 +30355,7 @@
       </c>
       <c r="AE254" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="255" spans="2:32" s="131" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -30974,7 +30974,7 @@
       </c>
       <c r="AE261" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>177.5</v>
+        <v>176.5</v>
       </c>
     </row>
     <row r="262" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -31064,7 +31064,7 @@
       </c>
       <c r="AE262" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="263" spans="2:32" s="131" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -31241,7 +31241,7 @@
       </c>
       <c r="AE264" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="265" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -31333,7 +31333,7 @@
       </c>
       <c r="AE265" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="266" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -31425,7 +31425,7 @@
       </c>
       <c r="AE266" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="267" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -31517,7 +31517,7 @@
       </c>
       <c r="AE267" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="268" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -31609,7 +31609,7 @@
       </c>
       <c r="AE268" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>1695.25</v>
+        <v>1694.25</v>
       </c>
     </row>
     <row r="269" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -31701,7 +31701,7 @@
       </c>
       <c r="AE269" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>1695.25</v>
+        <v>1694.25</v>
       </c>
     </row>
     <row r="270" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -31793,7 +31793,7 @@
       </c>
       <c r="AE270" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>1695.25</v>
+        <v>1694.25</v>
       </c>
     </row>
     <row r="271" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -32221,7 +32221,7 @@
       </c>
       <c r="AE275" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>542.75</v>
+        <v>541.75</v>
       </c>
     </row>
     <row r="276" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -32313,7 +32313,7 @@
       </c>
       <c r="AE276" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>51.625</v>
+        <v>50.625</v>
       </c>
     </row>
     <row r="277" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -32403,7 +32403,7 @@
       </c>
       <c r="AE277" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>51.625</v>
+        <v>50.625</v>
       </c>
     </row>
     <row r="278" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -32495,7 +32495,7 @@
       </c>
       <c r="AE278" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>51.625</v>
+        <v>50.625</v>
       </c>
     </row>
     <row r="279" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -32581,7 +32581,7 @@
       </c>
       <c r="AE279" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>177.5</v>
+        <v>176.5</v>
       </c>
     </row>
     <row r="280" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -32667,7 +32667,7 @@
       </c>
       <c r="AE280" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>177.5</v>
+        <v>176.5</v>
       </c>
     </row>
     <row r="281" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -32753,7 +32753,7 @@
       </c>
       <c r="AE281" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>177.5</v>
+        <v>176.5</v>
       </c>
     </row>
     <row r="282" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -32839,7 +32839,7 @@
       </c>
       <c r="AE282" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>177.5</v>
+        <v>176.5</v>
       </c>
     </row>
     <row r="283" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -32925,7 +32925,7 @@
       </c>
       <c r="AE283" s="71">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>-187.75</v>
+        <v>-188.75</v>
       </c>
       <c r="AF283" s="108" t="s">
         <v>107</v>
@@ -33016,7 +33016,7 @@
       </c>
       <c r="AE284" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>1695.25</v>
+        <v>1694.25</v>
       </c>
     </row>
     <row r="285" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -33274,7 +33274,7 @@
       </c>
       <c r="AE287" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>60.25</v>
+        <v>59.25</v>
       </c>
     </row>
     <row r="288" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -33368,7 +33368,7 @@
       </c>
       <c r="AE288" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="289" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -33460,7 +33460,7 @@
       </c>
       <c r="AE289" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="290" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -33552,7 +33552,7 @@
       </c>
       <c r="AE290" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="291" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -33644,7 +33644,7 @@
       </c>
       <c r="AE291" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="292" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -33740,7 +33740,7 @@
       </c>
       <c r="AE292" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="293" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -33836,7 +33836,7 @@
       </c>
       <c r="AE293" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="294" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -33932,7 +33932,7 @@
       </c>
       <c r="AE294" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="295" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -34028,7 +34028,7 @@
       </c>
       <c r="AE295" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="296" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -34124,7 +34124,7 @@
       </c>
       <c r="AE296" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="297" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -34311,7 +34311,7 @@
       </c>
       <c r="AE298" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="299" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -34407,7 +34407,7 @@
       </c>
       <c r="AE299" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="300" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -34503,7 +34503,7 @@
       </c>
       <c r="AE300" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="301" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -34599,7 +34599,7 @@
       </c>
       <c r="AE301" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="302" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -34695,7 +34695,7 @@
       </c>
       <c r="AE302" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="303" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -34791,7 +34791,7 @@
       </c>
       <c r="AE303" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="304" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -34887,7 +34887,7 @@
       </c>
       <c r="AE304" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="305" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -34983,7 +34983,7 @@
       </c>
       <c r="AE305" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="306" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -35079,7 +35079,7 @@
       </c>
       <c r="AE306" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="307" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -35175,7 +35175,7 @@
       </c>
       <c r="AE307" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="308" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -35271,7 +35271,7 @@
       </c>
       <c r="AE308" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="309" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -35367,7 +35367,7 @@
       </c>
       <c r="AE309" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="310" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -35463,7 +35463,7 @@
       </c>
       <c r="AE310" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="311" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -35561,7 +35561,7 @@
       </c>
       <c r="AE311" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="312" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -35659,7 +35659,7 @@
       </c>
       <c r="AE312" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="313" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -35755,7 +35755,7 @@
       </c>
       <c r="AE313" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="314" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -35851,7 +35851,7 @@
       </c>
       <c r="AE314" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="315" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -35949,7 +35949,7 @@
       </c>
       <c r="AE315" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="316" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -36045,7 +36045,7 @@
       </c>
       <c r="AE316" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="317" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -36141,7 +36141,7 @@
       </c>
       <c r="AE317" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="318" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -36239,7 +36239,7 @@
       </c>
       <c r="AE318" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="319" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -36335,7 +36335,7 @@
       </c>
       <c r="AE319" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="320" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -36431,7 +36431,7 @@
       </c>
       <c r="AE320" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="321" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -36527,7 +36527,7 @@
       </c>
       <c r="AE321" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="322" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -36623,7 +36623,7 @@
       </c>
       <c r="AE322" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="323" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -36719,7 +36719,7 @@
       </c>
       <c r="AE323" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="324" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -36815,7 +36815,7 @@
       </c>
       <c r="AE324" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="325" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -36911,7 +36911,7 @@
       </c>
       <c r="AE325" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="326" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -37009,7 +37009,7 @@
       </c>
       <c r="AE326" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="327" spans="2:32" s="131" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -38005,7 +38005,7 @@
       </c>
       <c r="AE337" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>177.5</v>
+        <v>176.5</v>
       </c>
     </row>
     <row r="338" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -38091,7 +38091,7 @@
       </c>
       <c r="AE338" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>177.5</v>
+        <v>176.5</v>
       </c>
     </row>
     <row r="339" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -38674,7 +38674,7 @@
       </c>
       <c r="AE345" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="346" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -38764,7 +38764,7 @@
       </c>
       <c r="AE346" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>51.625</v>
+        <v>50.625</v>
       </c>
     </row>
     <row r="347" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -38854,7 +38854,7 @@
       </c>
       <c r="AE347" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>234.25</v>
+        <v>233.25</v>
       </c>
     </row>
     <row r="348" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -38944,7 +38944,7 @@
       </c>
       <c r="AE348" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>51.625</v>
+        <v>50.625</v>
       </c>
     </row>
     <row r="349" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -39036,7 +39036,7 @@
       </c>
       <c r="AE349" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="350" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -39128,7 +39128,7 @@
       </c>
       <c r="AE350" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="351" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -39220,7 +39220,7 @@
       </c>
       <c r="AE351" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="352" spans="2:31" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -39312,7 +39312,7 @@
       </c>
       <c r="AE352" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="353" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -39398,7 +39398,7 @@
       </c>
       <c r="AE353" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="354" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -39486,7 +39486,7 @@
       </c>
       <c r="AE354" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="355" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -39578,7 +39578,7 @@
       </c>
       <c r="AE355" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="356" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -39668,7 +39668,7 @@
       </c>
       <c r="AE356" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="357" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -39758,7 +39758,7 @@
       </c>
       <c r="AE357" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="358" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -39848,7 +39848,7 @@
       </c>
       <c r="AE358" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="359" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -39920,7 +39920,7 @@
       </c>
       <c r="AE359" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="AF359" t="s">
         <v>1336</v>
@@ -39995,7 +39995,7 @@
       </c>
       <c r="AE360" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>692.125</v>
+        <v>691.125</v>
       </c>
       <c r="AF360" t="s">
         <v>1341</v>
@@ -40174,7 +40174,7 @@
       </c>
       <c r="AE362" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>51.625</v>
+        <v>50.625</v>
       </c>
     </row>
     <row r="363" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -40354,7 +40354,7 @@
       </c>
       <c r="AE364" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>51.625</v>
+        <v>50.625</v>
       </c>
     </row>
     <row r="365" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -40448,7 +40448,7 @@
       </c>
       <c r="AE365" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>51.625</v>
+        <v>50.625</v>
       </c>
     </row>
     <row r="366" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -41755,7 +41755,7 @@
       </c>
       <c r="AE380" s="54">
         <f ca="1">IF(Таблица1[[#This Row],[Next CAL]]="---","---",Таблица1[[#This Row],[Next CAL]]-$U$1)</f>
-        <v>146.5</v>
+        <v>145.5</v>
       </c>
     </row>
     <row r="381" spans="2:32" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -49249,16 +49249,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="T2:V2"/>
     <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="AC4:AD471">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="between">

</xml_diff>